<commit_message>
add summary of spearman
</commit_message>
<xml_diff>
--- a/biorefineries/wwt/results/uncertainties/oc2g_exist_100.xlsx
+++ b/biorefineries/wwt/results/uncertainties/oc2g_exist_100.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yalin\Dropbox\Li-Guest_Shared\Papers\5. Small-Footprint WWT\Temp data transfer\uncertainties\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yalinli_cabbi/Coding/bp/biorefineries/wwt/results/uncertainties/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF6E1FB1-F001-4757-8644-EC1E69C2B393}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98566667-9715-7B47-A5D0-EE8B77AA911F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="1350" windowWidth="21640" windowHeight="13780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="340" yWindow="1360" windowWidth="21640" windowHeight="13780" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -397,8 +397,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -747,9 +750,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -759,117 +762,117 @@
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2"/>
+      <c r="G1" s="3"/>
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
       <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2" t="s">
+      <c r="N1" s="3"/>
+      <c r="O1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2" t="s">
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="2"/>
+      <c r="R1" s="3"/>
       <c r="S1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2" t="s">
+      <c r="U1" s="3"/>
+      <c r="V1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2" t="s">
+      <c r="W1" s="3"/>
+      <c r="X1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Y1" s="2"/>
+      <c r="Y1" s="3"/>
       <c r="Z1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AA1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="AB1" s="2"/>
-      <c r="AC1" s="2" t="s">
+      <c r="AB1" s="3"/>
+      <c r="AC1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="AD1" s="2"/>
-      <c r="AE1" s="2" t="s">
+      <c r="AD1" s="3"/>
+      <c r="AE1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="AF1" s="2"/>
+      <c r="AF1" s="3"/>
       <c r="AG1" s="1" t="s">
         <v>20</v>
       </c>
       <c r="AH1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AI1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="AJ1" s="2"/>
-      <c r="AK1" s="2" t="s">
+      <c r="AJ1" s="3"/>
+      <c r="AK1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="AL1" s="2"/>
+      <c r="AL1" s="3"/>
       <c r="AM1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AN1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AO1" s="2"/>
+      <c r="AO1" s="3"/>
       <c r="AP1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="AQ1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AR1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AS1" s="2"/>
-      <c r="AT1" s="2" t="s">
+      <c r="AS1" s="3"/>
+      <c r="AT1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AU1" s="2"/>
-      <c r="AV1" s="2" t="s">
+      <c r="AU1" s="3"/>
+      <c r="AV1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AW1" s="2"/>
-      <c r="AX1" s="2"/>
-      <c r="AY1" s="2"/>
-      <c r="AZ1" s="2" t="s">
+      <c r="AW1" s="3"/>
+      <c r="AX1" s="3"/>
+      <c r="AY1" s="3"/>
+      <c r="AZ1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="BA1" s="2"/>
-      <c r="BB1" s="2"/>
-      <c r="BC1" s="2"/>
-      <c r="BD1" s="2"/>
+      <c r="BA1" s="3"/>
+      <c r="BB1" s="3"/>
+      <c r="BC1" s="3"/>
+      <c r="BD1" s="3"/>
     </row>
-    <row r="2" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1039,7 +1042,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -1209,7 +1212,7 @@
         <v>0.68225104634567912</v>
       </c>
     </row>
-    <row r="5" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -1379,7 +1382,7 @@
         <v>0.81580104406368481</v>
       </c>
     </row>
-    <row r="6" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -1549,7 +1552,7 @@
         <v>0.61429478034808804</v>
       </c>
     </row>
-    <row r="7" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -1719,7 +1722,7 @@
         <v>0.83186059053805539</v>
       </c>
     </row>
-    <row r="8" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -1889,7 +1892,7 @@
         <v>0.64927811630087418</v>
       </c>
     </row>
-    <row r="9" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>5</v>
       </c>
@@ -2059,7 +2062,7 @@
         <v>0.83672024904963083</v>
       </c>
     </row>
-    <row r="10" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>6</v>
       </c>
@@ -2229,7 +2232,7 @@
         <v>0.76526215835571254</v>
       </c>
     </row>
-    <row r="11" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>7</v>
       </c>
@@ -2399,7 +2402,7 @@
         <v>0.60532228503213048</v>
       </c>
     </row>
-    <row r="12" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>8</v>
       </c>
@@ -2569,7 +2572,7 @@
         <v>0.82938154529062524</v>
       </c>
     </row>
-    <row r="13" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>9</v>
       </c>
@@ -2739,7 +2742,7 @@
         <v>0.74171434865047181</v>
       </c>
     </row>
-    <row r="14" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>10</v>
       </c>
@@ -2909,7 +2912,7 @@
         <v>0.70258666946145287</v>
       </c>
     </row>
-    <row r="15" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>11</v>
       </c>
@@ -3079,7 +3082,7 @@
         <v>0.78997280232953071</v>
       </c>
     </row>
-    <row r="16" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>12</v>
       </c>
@@ -3249,7 +3252,7 @@
         <v>0.85200157935046739</v>
       </c>
     </row>
-    <row r="17" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>13</v>
       </c>
@@ -3419,7 +3422,7 @@
         <v>0.84650639046743481</v>
       </c>
     </row>
-    <row r="18" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>14</v>
       </c>
@@ -3589,7 +3592,7 @@
         <v>0.64272130707154407</v>
       </c>
     </row>
-    <row r="19" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>15</v>
       </c>
@@ -3759,7 +3762,7 @@
         <v>0.66214052382379518</v>
       </c>
     </row>
-    <row r="20" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -3929,7 +3932,7 @@
         <v>0.81432204211834824</v>
       </c>
     </row>
-    <row r="21" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -4099,7 +4102,7 @@
         <v>0.79333386009521267</v>
       </c>
     </row>
-    <row r="22" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -4269,7 +4272,7 @@
         <v>0.70824680337987889</v>
       </c>
     </row>
-    <row r="23" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>19</v>
       </c>
@@ -4439,7 +4442,7 @@
         <v>0.63485304785408836</v>
       </c>
     </row>
-    <row r="24" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>20</v>
       </c>
@@ -4609,7 +4612,7 @@
         <v>0.62047597009617406</v>
       </c>
     </row>
-    <row r="25" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>21</v>
       </c>
@@ -4779,7 +4782,7 @@
         <v>0.84087800993271011</v>
       </c>
     </row>
-    <row r="26" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>22</v>
       </c>
@@ -4949,7 +4952,7 @@
         <v>0.57001248783600134</v>
       </c>
     </row>
-    <row r="27" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>23</v>
       </c>
@@ -5119,7 +5122,7 @@
         <v>0.53860969307564632</v>
       </c>
     </row>
-    <row r="28" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>24</v>
       </c>
@@ -5289,7 +5292,7 @@
         <v>0.7720171866702481</v>
       </c>
     </row>
-    <row r="29" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>25</v>
       </c>
@@ -5459,7 +5462,7 @@
         <v>0.65423838902672149</v>
       </c>
     </row>
-    <row r="30" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>26</v>
       </c>
@@ -5629,7 +5632,7 @@
         <v>0.86480071833023309</v>
       </c>
     </row>
-    <row r="31" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>27</v>
       </c>
@@ -5799,7 +5802,7 @@
         <v>0.71093547687742764</v>
       </c>
     </row>
-    <row r="32" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>28</v>
       </c>
@@ -5969,7 +5972,7 @@
         <v>0.64609881894185828</v>
       </c>
     </row>
-    <row r="33" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>29</v>
       </c>
@@ -6139,7 +6142,7 @@
         <v>0.74641421802346075</v>
       </c>
     </row>
-    <row r="34" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>30</v>
       </c>
@@ -6309,7 +6312,7 @@
         <v>0.83425642525687471</v>
       </c>
     </row>
-    <row r="35" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>31</v>
       </c>
@@ -6479,7 +6482,7 @@
         <v>0.86153509526783711</v>
       </c>
     </row>
-    <row r="36" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>32</v>
       </c>
@@ -6649,7 +6652,7 @@
         <v>0.80945296918811549</v>
       </c>
     </row>
-    <row r="37" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>33</v>
       </c>
@@ -6819,7 +6822,7 @@
         <v>0.58055307538490275</v>
       </c>
     </row>
-    <row r="38" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>34</v>
       </c>
@@ -6989,7 +6992,7 @@
         <v>0.8254838427614507</v>
       </c>
     </row>
-    <row r="39" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>35</v>
       </c>
@@ -7159,7 +7162,7 @@
         <v>0.76172768929107015</v>
       </c>
     </row>
-    <row r="40" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>36</v>
       </c>
@@ -7329,7 +7332,7 @@
         <v>0.68901671698303735</v>
       </c>
     </row>
-    <row r="41" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>37</v>
       </c>
@@ -7499,7 +7502,7 @@
         <v>0.72796127573438252</v>
       </c>
     </row>
-    <row r="42" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>38</v>
       </c>
@@ -7669,7 +7672,7 @@
         <v>0.75642945354883429</v>
       </c>
     </row>
-    <row r="43" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>39</v>
       </c>
@@ -7839,7 +7842,7 @@
         <v>0.55747389656880075</v>
       </c>
     </row>
-    <row r="44" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>40</v>
       </c>
@@ -8009,7 +8012,7 @@
         <v>0.79668895297202613</v>
       </c>
     </row>
-    <row r="45" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>41</v>
       </c>
@@ -8179,7 +8182,7 @@
         <v>0.68400647595518127</v>
       </c>
     </row>
-    <row r="46" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>42</v>
       </c>
@@ -8349,7 +8352,7 @@
         <v>0.57502385479059437</v>
       </c>
     </row>
-    <row r="47" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>43</v>
       </c>
@@ -8519,7 +8522,7 @@
         <v>0.78531039290957849</v>
       </c>
     </row>
-    <row r="48" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>44</v>
       </c>
@@ -8689,7 +8692,7 @@
         <v>0.87267282158682002</v>
       </c>
     </row>
-    <row r="49" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>45</v>
       </c>
@@ -8859,7 +8862,7 @@
         <v>0.74937575718757088</v>
       </c>
     </row>
-    <row r="50" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>46</v>
       </c>
@@ -9029,7 +9032,7 @@
         <v>0.58725890111834556</v>
       </c>
     </row>
-    <row r="51" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>47</v>
       </c>
@@ -9199,7 +9202,7 @@
         <v>0.60606239125559069</v>
       </c>
     </row>
-    <row r="52" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>48</v>
       </c>
@@ -9369,7 +9372,7 @@
         <v>0.72229293356868562</v>
       </c>
     </row>
-    <row r="53" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>49</v>
       </c>
@@ -9539,7 +9542,7 @@
         <v>0.62758358985770746</v>
       </c>
     </row>
-    <row r="54" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>50</v>
       </c>
@@ -9709,7 +9712,7 @@
         <v>0.5710181282649387</v>
       </c>
     </row>
-    <row r="55" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>51</v>
       </c>
@@ -9879,7 +9882,7 @@
         <v>0.6914974848036799</v>
       </c>
     </row>
-    <row r="56" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>52</v>
       </c>
@@ -10049,7 +10052,7 @@
         <v>0.78067588303234059</v>
       </c>
     </row>
-    <row r="57" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>53</v>
       </c>
@@ -10219,7 +10222,7 @@
         <v>0.62549784456606505</v>
       </c>
     </row>
-    <row r="58" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>54</v>
       </c>
@@ -10389,7 +10392,7 @@
         <v>0.69752273324931879</v>
       </c>
     </row>
-    <row r="59" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>55</v>
       </c>
@@ -10559,7 +10562,7 @@
         <v>0.55471498609717163</v>
       </c>
     </row>
-    <row r="60" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>56</v>
       </c>
@@ -10729,7 +10732,7 @@
         <v>0.85842557274567666</v>
       </c>
     </row>
-    <row r="61" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>57</v>
       </c>
@@ -10899,7 +10902,7 @@
         <v>0.526277977208506</v>
       </c>
     </row>
-    <row r="62" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>58</v>
       </c>
@@ -11069,7 +11072,7 @@
         <v>0.52919496365096341</v>
       </c>
     </row>
-    <row r="63" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>59</v>
       </c>
@@ -11239,7 +11242,7 @@
         <v>0.53358131802622388</v>
       </c>
     </row>
-    <row r="64" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>60</v>
       </c>
@@ -11409,7 +11412,7 @@
         <v>0.74520751310037958</v>
       </c>
     </row>
-    <row r="65" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>61</v>
       </c>
@@ -11579,7 +11582,7 @@
         <v>0.67319946196757163</v>
       </c>
     </row>
-    <row r="66" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>62</v>
       </c>
@@ -11749,7 +11752,7 @@
         <v>0.73382271503164875</v>
       </c>
     </row>
-    <row r="67" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>63</v>
       </c>
@@ -11919,7 +11922,7 @@
         <v>0.59810290411945688</v>
       </c>
     </row>
-    <row r="68" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>64</v>
       </c>
@@ -12089,7 +12092,7 @@
         <v>0.59207951934212288</v>
       </c>
     </row>
-    <row r="69" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>65</v>
       </c>
@@ -12259,7 +12262,7 @@
         <v>0.70486446868268071</v>
       </c>
     </row>
-    <row r="70" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>66</v>
       </c>
@@ -12429,7 +12432,7 @@
         <v>0.63276618843746024</v>
       </c>
     </row>
-    <row r="71" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>67</v>
       </c>
@@ -12599,7 +12602,7 @@
         <v>0.75557721179375992</v>
       </c>
     </row>
-    <row r="72" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>68</v>
       </c>
@@ -12769,7 +12772,7 @@
         <v>0.66062889452449036</v>
       </c>
     </row>
-    <row r="73" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>69</v>
       </c>
@@ -12939,7 +12942,7 @@
         <v>0.8022616535417042</v>
       </c>
     </row>
-    <row r="74" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>70</v>
       </c>
@@ -13109,7 +13112,7 @@
         <v>0.54637453424062887</v>
       </c>
     </row>
-    <row r="75" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>71</v>
       </c>
@@ -13279,7 +13282,7 @@
         <v>0.55104413608660285</v>
       </c>
     </row>
-    <row r="76" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>72</v>
       </c>
@@ -13449,7 +13452,7 @@
         <v>0.63920825592816688</v>
       </c>
     </row>
-    <row r="77" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>73</v>
       </c>
@@ -13619,7 +13622,7 @@
         <v>0.71817873818926026</v>
       </c>
     </row>
-    <row r="78" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>74</v>
       </c>
@@ -13789,7 +13792,7 @@
         <v>0.8068005596452672</v>
       </c>
     </row>
-    <row r="79" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>75</v>
       </c>
@@ -13959,7 +13962,7 @@
         <v>0.58276530228756784</v>
       </c>
     </row>
-    <row r="80" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>76</v>
       </c>
@@ -14129,7 +14132,7 @@
         <v>0.77794795707288134</v>
       </c>
     </row>
-    <row r="81" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>77</v>
       </c>
@@ -14299,7 +14302,7 @@
         <v>0.77469276002784548</v>
       </c>
     </row>
-    <row r="82" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>78</v>
       </c>
@@ -14469,7 +14472,7 @@
         <v>0.61007859616319737</v>
       </c>
     </row>
-    <row r="83" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>79</v>
       </c>
@@ -14639,7 +14642,7 @@
         <v>0.58801789377592006</v>
       </c>
     </row>
-    <row r="84" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>80</v>
       </c>
@@ -14809,7 +14812,7 @@
         <v>0.6774140670528197</v>
       </c>
     </row>
-    <row r="85" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>81</v>
       </c>
@@ -14979,7 +14982,7 @@
         <v>0.65631176289754301</v>
       </c>
     </row>
-    <row r="86" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>82</v>
       </c>
@@ -15149,7 +15152,7 @@
         <v>0.85733950464569253</v>
       </c>
     </row>
-    <row r="87" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>83</v>
       </c>
@@ -15319,7 +15322,7 @@
         <v>0.60189242077076921</v>
       </c>
     </row>
-    <row r="88" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>84</v>
       </c>
@@ -15489,7 +15492,7 @@
         <v>0.73087931425523534</v>
       </c>
     </row>
-    <row r="89" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>85</v>
       </c>
@@ -15659,7 +15662,7 @@
         <v>0.56503132570384162</v>
       </c>
     </row>
-    <row r="90" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>86</v>
       </c>
@@ -15829,7 +15832,7 @@
         <v>0.69395361115886545</v>
       </c>
     </row>
-    <row r="91" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>87</v>
       </c>
@@ -15999,7 +16002,7 @@
         <v>0.73564593143330748</v>
       </c>
     </row>
-    <row r="92" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>88</v>
       </c>
@@ -16169,7 +16172,7 @@
         <v>0.87143448525560196</v>
       </c>
     </row>
-    <row r="93" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>89</v>
       </c>
@@ -16339,7 +16342,7 @@
         <v>0.56330572324265626</v>
       </c>
     </row>
-    <row r="94" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>90</v>
       </c>
@@ -16509,7 +16512,7 @@
         <v>0.54485203133739435</v>
       </c>
     </row>
-    <row r="95" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>91</v>
       </c>
@@ -16679,7 +16682,7 @@
         <v>0.66506676133438702</v>
       </c>
     </row>
-    <row r="96" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>92</v>
       </c>
@@ -16849,7 +16852,7 @@
         <v>0.54014852045411499</v>
       </c>
     </row>
-    <row r="97" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>93</v>
       </c>
@@ -17019,7 +17022,7 @@
         <v>0.76841741363289073</v>
       </c>
     </row>
-    <row r="98" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>94</v>
       </c>
@@ -17189,7 +17192,7 @@
         <v>0.81993886736853228</v>
       </c>
     </row>
-    <row r="99" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>95</v>
       </c>
@@ -17359,7 +17362,7 @@
         <v>0.71698009751245728</v>
       </c>
     </row>
-    <row r="100" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>96</v>
       </c>
@@ -17529,7 +17532,7 @@
         <v>0.79800730884085991</v>
       </c>
     </row>
-    <row r="101" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>97</v>
       </c>
@@ -17699,7 +17702,7 @@
         <v>0.85006816520205786</v>
       </c>
     </row>
-    <row r="102" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>98</v>
       </c>
@@ -17869,7 +17872,7 @@
         <v>0.61795412962363194</v>
       </c>
     </row>
-    <row r="103" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>99</v>
       </c>
@@ -18041,6 +18044,16 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="AA1:AB1"/>
     <mergeCell ref="AR1:AS1"/>
     <mergeCell ref="AT1:AU1"/>
     <mergeCell ref="AV1:AY1"/>
@@ -18050,16 +18063,6 @@
     <mergeCell ref="AI1:AJ1"/>
     <mergeCell ref="AK1:AL1"/>
     <mergeCell ref="AN1:AO1"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="AA1:AB1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18069,40 +18072,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -18158,7 +18161,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -18211,7 +18214,7 @@
         <v>0.1003401904775096</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -18264,7 +18267,7 @@
         <v>0.14771093801085111</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -18317,7 +18320,7 @@
         <v>9.2126092150297573E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -18370,7 +18373,7 @@
         <v>0.12792124041131531</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -18423,7 +18426,7 @@
         <v>0.16788125867900761</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>5</v>
       </c>
@@ -18476,7 +18479,7 @@
         <v>0.2124192359496683</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>6</v>
       </c>
@@ -18529,12 +18532,12 @@
         <v>0.18885323421148359</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>8</v>
       </c>
@@ -18587,7 +18590,7 @@
         <v>0.1560363445762539</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>9</v>
       </c>
@@ -18640,7 +18643,7 @@
         <v>0.14813649276852051</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>10</v>
       </c>
@@ -18693,7 +18696,7 @@
         <v>9.5025590299193344E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>11</v>
       </c>
@@ -18746,7 +18749,7 @@
         <v>0.13550329585908241</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>12</v>
       </c>
@@ -18799,7 +18802,7 @@
         <v>0.2111128591636503</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>13</v>
       </c>
@@ -18852,12 +18855,12 @@
         <v>0.16216330057102221</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>15</v>
       </c>
@@ -18910,7 +18913,7 @@
         <v>0.22684399283769241</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -18963,7 +18966,7 @@
         <v>0.17901740747656539</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -19016,7 +19019,7 @@
         <v>0.10449771543471691</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -19069,7 +19072,7 @@
         <v>0.2743069571236858</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>19</v>
       </c>
@@ -19122,22 +19125,22 @@
         <v>8.3028814784920302E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>23</v>
       </c>
@@ -19190,7 +19193,7 @@
         <v>0.2009740055073273</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>24</v>
       </c>
@@ -19243,7 +19246,7 @@
         <v>0.26265842995032918</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>25</v>
       </c>
@@ -19296,7 +19299,7 @@
         <v>9.3990636130204266E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>26</v>
       </c>
@@ -19349,12 +19352,12 @@
         <v>0.14697728660362841</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>28</v>
       </c>
@@ -19407,7 +19410,7 @@
         <v>0.1225144100843169</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>29</v>
       </c>
@@ -19460,12 +19463,12 @@
         <v>0.23081224152966209</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>31</v>
       </c>
@@ -19518,7 +19521,7 @@
         <v>9.3548284717783911E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>32</v>
       </c>
@@ -19571,7 +19574,7 @@
         <v>0.1254756481945265</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>33</v>
       </c>
@@ -19624,7 +19627,7 @@
         <v>0.21575216817004819</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>34</v>
       </c>
@@ -19677,7 +19680,7 @@
         <v>0.13671950810937589</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>35</v>
       </c>
@@ -19730,7 +19733,7 @@
         <v>0.1092833876121287</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>36</v>
       </c>
@@ -19783,7 +19786,7 @@
         <v>0.15728321627368491</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>37</v>
       </c>
@@ -19836,7 +19839,7 @@
         <v>0.24352283901274091</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>38</v>
       </c>
@@ -19889,7 +19892,7 @@
         <v>0.19870870456991799</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>39</v>
       </c>
@@ -19942,7 +19945,7 @@
         <v>0.14364989811362741</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>40</v>
       </c>
@@ -19995,12 +19998,12 @@
         <v>0.12772077538916329</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>42</v>
       </c>
@@ -20053,7 +20056,7 @@
         <v>0.10091229962882881</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>43</v>
       </c>
@@ -20106,7 +20109,7 @@
         <v>0.1032139681166943</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>44</v>
       </c>
@@ -20159,7 +20162,7 @@
         <v>8.9990308588674212E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>45</v>
       </c>
@@ -20212,7 +20215,7 @@
         <v>0.101579578422552</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>46</v>
       </c>
@@ -20265,7 +20268,7 @@
         <v>0.1179680789376872</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>47</v>
       </c>
@@ -20318,7 +20321,7 @@
         <v>0.16788377491993739</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>48</v>
       </c>
@@ -20371,7 +20374,7 @@
         <v>0.14013253646281601</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>49</v>
       </c>
@@ -20424,7 +20427,7 @@
         <v>0.1622098128033512</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>50</v>
       </c>
@@ -20477,7 +20480,7 @@
         <v>0.11236381517047001</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>51</v>
       </c>
@@ -20530,12 +20533,12 @@
         <v>9.4578293732735477E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>52</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>53</v>
       </c>
@@ -20588,7 +20591,7 @@
         <v>0.1139088904661661</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>54</v>
       </c>
@@ -20641,12 +20644,12 @@
         <v>0.1680894637725332</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>55</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>56</v>
       </c>
@@ -20699,7 +20702,7 @@
         <v>0.17684571587373221</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>57</v>
       </c>
@@ -20752,7 +20755,7 @@
         <v>0.23216099233799001</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>58</v>
       </c>
@@ -20805,7 +20808,7 @@
         <v>0.188498363572424</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>59</v>
       </c>
@@ -20858,7 +20861,7 @@
         <v>0.1816704030786041</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>60</v>
       </c>
@@ -20911,7 +20914,7 @@
         <v>0.1276580113156657</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>61</v>
       </c>
@@ -20964,7 +20967,7 @@
         <v>0.1006830022692239</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>62</v>
       </c>
@@ -21017,7 +21020,7 @@
         <v>0.19729022844511801</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>63</v>
       </c>
@@ -21070,7 +21073,7 @@
         <v>0.17266344025956221</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>64</v>
       </c>
@@ -21123,7 +21126,7 @@
         <v>0.17435696669449879</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>65</v>
       </c>
@@ -21176,7 +21179,7 @@
         <v>0.1983227017475078</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>66</v>
       </c>
@@ -21229,7 +21232,7 @@
         <v>0.14117684281039611</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>67</v>
       </c>
@@ -21282,7 +21285,7 @@
         <v>0.1234837073662962</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>68</v>
       </c>
@@ -21335,7 +21338,7 @@
         <v>0.2679768582242868</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>69</v>
       </c>
@@ -21388,7 +21391,7 @@
         <v>0.1048487105948102</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>70</v>
       </c>
@@ -21441,7 +21444,7 @@
         <v>0.2051699364951759</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>71</v>
       </c>
@@ -21494,7 +21497,7 @@
         <v>9.0102274845784244E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>72</v>
       </c>
@@ -21547,22 +21550,22 @@
         <v>0.14411356825324159</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>73</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>74</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>75</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>76</v>
       </c>
@@ -21615,12 +21618,12 @@
         <v>0.11234661590411869</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>77</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>78</v>
       </c>
@@ -21673,7 +21676,7 @@
         <v>0.12408589670803261</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>79</v>
       </c>
@@ -21726,12 +21729,12 @@
         <v>0.1610423628942261</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>80</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>81</v>
       </c>
@@ -21784,7 +21787,7 @@
         <v>0.1581055050705239</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>82</v>
       </c>
@@ -21837,7 +21840,7 @@
         <v>0.11622875274421821</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>83</v>
       </c>
@@ -21890,7 +21893,7 @@
         <v>0.14220681913133809</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>84</v>
       </c>
@@ -21943,7 +21946,7 @@
         <v>0.1149483015808594</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>85</v>
       </c>
@@ -21996,7 +21999,7 @@
         <v>0.1118161581911726</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>86</v>
       </c>
@@ -22049,7 +22052,7 @@
         <v>0.20812621466964801</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>87</v>
       </c>
@@ -22102,7 +22105,7 @@
         <v>0.1022603319243419</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>88</v>
       </c>
@@ -22155,7 +22158,7 @@
         <v>0.21790701206565419</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>89</v>
       </c>
@@ -22208,7 +22211,7 @@
         <v>0.18663929758296821</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>90</v>
       </c>
@@ -22261,7 +22264,7 @@
         <v>0.14301576873436739</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>91</v>
       </c>
@@ -22314,7 +22317,7 @@
         <v>0.1005257080430314</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>92</v>
       </c>
@@ -22367,7 +22370,7 @@
         <v>9.6315755367863701E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>93</v>
       </c>
@@ -22420,7 +22423,7 @@
         <v>9.8490784235466949E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>94</v>
       </c>
@@ -22473,7 +22476,7 @@
         <v>0.17179850904250879</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>95</v>
       </c>
@@ -22526,7 +22529,7 @@
         <v>0.2234466857253809</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>96</v>
       </c>
@@ -22579,7 +22582,7 @@
         <v>0.19210161020711361</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>97</v>
       </c>
@@ -22632,12 +22635,12 @@
         <v>0.19378256717234951</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>98</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>99</v>
       </c>
@@ -22704,33 +22707,33 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -22786,7 +22789,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -22839,7 +22842,7 @@
         <v>8.3028814784920302E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>0.05</v>
       </c>
@@ -22892,7 +22895,7 @@
         <v>9.3614637429646971E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>0.25</v>
       </c>
@@ -22945,7 +22948,7 @@
         <v>0.1122140014758822</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>0.5</v>
       </c>
@@ -22998,7 +23001,7 @@
         <v>0.14554542742843499</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>0.75</v>
       </c>
@@ -23051,7 +23054,7 @@
         <v>0.1885870812321889</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>0.95</v>
       </c>
@@ -23104,7 +23107,7 @@
         <v>0.23195867971674081</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -23169,11 +23172,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:S56"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -23183,7 +23188,7 @@
       <c r="C1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>88</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -23232,7 +23237,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -23288,7 +23293,7 @@
         <v>-6.6659916978839731E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -23344,8 +23349,8 @@
         <v>3.4018426647767549E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -23400,8 +23405,8 @@
         <v>5.7669332793358313E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A5" s="2"/>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
       <c r="B5" s="1" t="s">
         <v>34</v>
       </c>
@@ -23454,8 +23459,8 @@
         <v>0.17813101144072091</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -23510,8 +23515,8 @@
         <v>-7.9659815733522335E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A7" s="2"/>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
       <c r="B7" s="1" t="s">
         <v>36</v>
       </c>
@@ -23564,7 +23569,7 @@
         <v>1.5956262022881439E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -23620,8 +23625,8 @@
         <v>0.13014073099119169</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -23676,8 +23681,8 @@
         <v>-7.552900678343627E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A10" s="2"/>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
       <c r="B10" s="1" t="s">
         <v>39</v>
       </c>
@@ -23730,8 +23735,8 @@
         <v>0.97195504707907265</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A11" s="2"/>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
       <c r="B11" s="1" t="s">
         <v>40</v>
       </c>
@@ -23784,7 +23789,7 @@
         <v>0.1441125847929533</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -23840,8 +23845,8 @@
         <v>-0.22913840234889141</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -23896,8 +23901,8 @@
         <v>-0.1113293510175155</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A14" s="2"/>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A14" s="3"/>
       <c r="B14" s="1" t="s">
         <v>43</v>
       </c>
@@ -23950,8 +23955,8 @@
         <v>1.480206540447504E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -24006,8 +24011,8 @@
         <v>-0.1006985926900881</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A16" s="2"/>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A16" s="3"/>
       <c r="B16" s="1" t="s">
         <v>45</v>
       </c>
@@ -24060,8 +24065,8 @@
         <v>1.5105801356687249E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -24116,8 +24121,8 @@
         <v>0.21976308595727451</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A18" s="2"/>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A18" s="3"/>
       <c r="B18" s="1" t="s">
         <v>47</v>
       </c>
@@ -24170,7 +24175,7 @@
         <v>5.8722284094360642E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>12</v>
       </c>
@@ -24226,8 +24231,8 @@
         <v>-5.7142857142857141E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -24282,8 +24287,8 @@
         <v>6.2569606155715302E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A21" s="2"/>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A21" s="3"/>
       <c r="B21" s="1" t="s">
         <v>50</v>
       </c>
@@ -24336,8 +24341,8 @@
         <v>6.906955553305659E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -24392,8 +24397,8 @@
         <v>0.1370861597651109</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A23" s="2"/>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A23" s="3"/>
       <c r="B23" s="1" t="s">
         <v>52</v>
       </c>
@@ -24446,8 +24451,8 @@
         <v>-9.4664371772805511E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -24502,8 +24507,8 @@
         <v>4.6167864736255948E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A25" s="2"/>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A25" s="3"/>
       <c r="B25" s="1" t="s">
         <v>54</v>
       </c>
@@ -24556,7 +24561,7 @@
         <v>-9.0148830616583991E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>16</v>
       </c>
@@ -24612,8 +24617,8 @@
         <v>-8.0267287637946744E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A27" s="2" t="s">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -24668,8 +24673,8 @@
         <v>-5.0359420876784453E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A28" s="2"/>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A28" s="3"/>
       <c r="B28" s="1" t="s">
         <v>57</v>
       </c>
@@ -24722,8 +24727,8 @@
         <v>-2.6931254429482642E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A29" s="2" t="s">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -24778,8 +24783,8 @@
         <v>0.11859876480712769</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A30" s="2"/>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A30" s="3"/>
       <c r="B30" s="1" t="s">
         <v>59</v>
       </c>
@@ -24832,8 +24837,8 @@
         <v>0.10906145590766431</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A31" s="2" t="s">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -24888,8 +24893,8 @@
         <v>-0.16932266882656671</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A32" s="2"/>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A32" s="3"/>
       <c r="B32" s="1" t="s">
         <v>61</v>
       </c>
@@ -24942,7 +24947,7 @@
         <v>-5.5543181127872841E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>20</v>
       </c>
@@ -24998,7 +25003,7 @@
         <v>-1.553103168978435E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>21</v>
       </c>
@@ -25054,8 +25059,8 @@
         <v>9.027032499746887E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A35" s="2" t="s">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -25110,8 +25115,8 @@
         <v>3.98906550572036E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A36" s="2"/>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A36" s="3"/>
       <c r="B36" s="1" t="s">
         <v>65</v>
       </c>
@@ -25164,8 +25169,8 @@
         <v>-4.3211501468057099E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A37" s="2" t="s">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -25220,8 +25225,8 @@
         <v>0.19844082211197731</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A38" s="2"/>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A38" s="3"/>
       <c r="B38" s="1" t="s">
         <v>67</v>
       </c>
@@ -25274,7 +25279,7 @@
         <v>-2.90371570314873E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>24</v>
       </c>
@@ -25330,8 +25335,8 @@
         <v>6.0159967601498429E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A40" s="2" t="s">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -25386,8 +25391,8 @@
         <v>0.1192669839019945</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A41" s="2"/>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A41" s="3"/>
       <c r="B41" s="1" t="s">
         <v>70</v>
       </c>
@@ -25440,7 +25445,7 @@
         <v>-6.0544699807633898E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>25</v>
       </c>
@@ -25496,7 +25501,7 @@
         <v>0.22265870203503091</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>26</v>
       </c>
@@ -25552,8 +25557,8 @@
         <v>-0.1239850156930242</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A44" s="2" t="s">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -25608,8 +25613,8 @@
         <v>8.8771894299888632E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A45" s="2"/>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A45" s="3"/>
       <c r="B45" s="1" t="s">
         <v>74</v>
       </c>
@@ -25662,8 +25667,8 @@
         <v>0.1449022982687051</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A46" s="2" t="s">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -25718,8 +25723,8 @@
         <v>3.1467044649184983E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A47" s="2"/>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A47" s="3"/>
       <c r="B47" s="1" t="s">
         <v>76</v>
       </c>
@@ -25772,8 +25777,8 @@
         <v>-3.8493469677027443E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A48" s="2" t="s">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -25828,8 +25833,8 @@
         <v>-0.20494077148931861</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A49" s="2"/>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A49" s="3"/>
       <c r="B49" s="1" t="s">
         <v>78</v>
       </c>
@@ -25882,8 +25887,8 @@
         <v>-2.6020046572846001E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A50" s="2"/>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A50" s="3"/>
       <c r="B50" s="1" t="s">
         <v>79</v>
       </c>
@@ -25936,8 +25941,8 @@
         <v>-5.8114812189936221E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A51" s="2"/>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A51" s="3"/>
       <c r="B51" s="1" t="s">
         <v>80</v>
       </c>
@@ -25990,8 +25995,8 @@
         <v>6.724713981978335E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A52" s="2" t="s">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -26046,8 +26051,8 @@
         <v>-0.1045459147514427</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A53" s="2"/>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A53" s="3"/>
       <c r="B53" s="1" t="s">
         <v>82</v>
       </c>
@@ -26100,8 +26105,8 @@
         <v>-3.7622759947352438E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A54" s="2"/>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A54" s="3"/>
       <c r="B54" s="1" t="s">
         <v>83</v>
       </c>
@@ -26154,8 +26159,8 @@
         <v>-5.0582160575073407E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A55" s="2"/>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A55" s="3"/>
       <c r="B55" s="1" t="s">
         <v>84</v>
       </c>
@@ -26208,8 +26213,8 @@
         <v>8.6767237015288032E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A56" s="2"/>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A56" s="3"/>
       <c r="B56" s="1" t="s">
         <v>85</v>
       </c>
@@ -26264,6 +26269,16 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A27:A28"/>
     <mergeCell ref="A44:A45"/>
     <mergeCell ref="A46:A47"/>
     <mergeCell ref="A48:A51"/>
@@ -26273,16 +26288,6 @@
     <mergeCell ref="A35:A36"/>
     <mergeCell ref="A37:A38"/>
     <mergeCell ref="A40:A41"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -26294,9 +26299,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:73" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -26306,136 +26311,136 @@
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2"/>
+      <c r="G1" s="3"/>
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
       <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2" t="s">
+      <c r="N1" s="3"/>
+      <c r="O1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2" t="s">
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="2"/>
+      <c r="R1" s="3"/>
       <c r="S1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2" t="s">
+      <c r="U1" s="3"/>
+      <c r="V1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2" t="s">
+      <c r="W1" s="3"/>
+      <c r="X1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Y1" s="2"/>
+      <c r="Y1" s="3"/>
       <c r="Z1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AA1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="AB1" s="2"/>
-      <c r="AC1" s="2" t="s">
+      <c r="AB1" s="3"/>
+      <c r="AC1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="AD1" s="2"/>
-      <c r="AE1" s="2" t="s">
+      <c r="AD1" s="3"/>
+      <c r="AE1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="AF1" s="2"/>
+      <c r="AF1" s="3"/>
       <c r="AG1" s="1" t="s">
         <v>20</v>
       </c>
       <c r="AH1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AI1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="AJ1" s="2"/>
-      <c r="AK1" s="2" t="s">
+      <c r="AJ1" s="3"/>
+      <c r="AK1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="AL1" s="2"/>
+      <c r="AL1" s="3"/>
       <c r="AM1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AN1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AO1" s="2"/>
+      <c r="AO1" s="3"/>
       <c r="AP1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="AQ1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AR1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AS1" s="2"/>
-      <c r="AT1" s="2" t="s">
+      <c r="AS1" s="3"/>
+      <c r="AT1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AU1" s="2"/>
-      <c r="AV1" s="2" t="s">
+      <c r="AU1" s="3"/>
+      <c r="AV1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AW1" s="2"/>
-      <c r="AX1" s="2"/>
-      <c r="AY1" s="2"/>
-      <c r="AZ1" s="2" t="s">
+      <c r="AW1" s="3"/>
+      <c r="AX1" s="3"/>
+      <c r="AY1" s="3"/>
+      <c r="AZ1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="BA1" s="2"/>
-      <c r="BB1" s="2"/>
-      <c r="BC1" s="2"/>
-      <c r="BD1" s="2"/>
-      <c r="BE1" s="2" t="s">
+      <c r="BA1" s="3"/>
+      <c r="BB1" s="3"/>
+      <c r="BC1" s="3"/>
+      <c r="BD1" s="3"/>
+      <c r="BE1" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="BF1" s="2"/>
-      <c r="BG1" s="2"/>
-      <c r="BH1" s="2"/>
-      <c r="BI1" s="2"/>
-      <c r="BJ1" s="2"/>
-      <c r="BK1" s="2"/>
-      <c r="BL1" s="2"/>
-      <c r="BM1" s="2"/>
-      <c r="BN1" s="2"/>
-      <c r="BO1" s="2"/>
-      <c r="BP1" s="2"/>
-      <c r="BQ1" s="2"/>
-      <c r="BR1" s="2"/>
-      <c r="BS1" s="2"/>
-      <c r="BT1" s="2"/>
-      <c r="BU1" s="2"/>
+      <c r="BF1" s="3"/>
+      <c r="BG1" s="3"/>
+      <c r="BH1" s="3"/>
+      <c r="BI1" s="3"/>
+      <c r="BJ1" s="3"/>
+      <c r="BK1" s="3"/>
+      <c r="BL1" s="3"/>
+      <c r="BM1" s="3"/>
+      <c r="BN1" s="3"/>
+      <c r="BO1" s="3"/>
+      <c r="BP1" s="3"/>
+      <c r="BQ1" s="3"/>
+      <c r="BR1" s="3"/>
+      <c r="BS1" s="3"/>
+      <c r="BT1" s="3"/>
+      <c r="BU1" s="3"/>
     </row>
-    <row r="2" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:73" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -26656,7 +26661,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:73" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -26874,7 +26879,7 @@
         <v>0.1003401904775096</v>
       </c>
     </row>
-    <row r="5" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:73" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -27092,7 +27097,7 @@
         <v>0.14771093801085111</v>
       </c>
     </row>
-    <row r="6" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:73" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -27310,7 +27315,7 @@
         <v>9.2126092150297573E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:73" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -27528,7 +27533,7 @@
         <v>0.12792124041131531</v>
       </c>
     </row>
-    <row r="8" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:73" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -27746,7 +27751,7 @@
         <v>0.16788125867900761</v>
       </c>
     </row>
-    <row r="9" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:73" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>5</v>
       </c>
@@ -27964,7 +27969,7 @@
         <v>0.2124192359496683</v>
       </c>
     </row>
-    <row r="10" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:73" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>6</v>
       </c>
@@ -28182,7 +28187,7 @@
         <v>0.18885323421148359</v>
       </c>
     </row>
-    <row r="11" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:73" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>7</v>
       </c>
@@ -28352,7 +28357,7 @@
         <v>0.60532228503213048</v>
       </c>
     </row>
-    <row r="12" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:73" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>8</v>
       </c>
@@ -28570,7 +28575,7 @@
         <v>0.1560363445762539</v>
       </c>
     </row>
-    <row r="13" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:73" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>9</v>
       </c>
@@ -28788,7 +28793,7 @@
         <v>0.14813649276852051</v>
       </c>
     </row>
-    <row r="14" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:73" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>10</v>
       </c>
@@ -29006,7 +29011,7 @@
         <v>9.5025590299193344E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:73" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>11</v>
       </c>
@@ -29224,7 +29229,7 @@
         <v>0.13550329585908241</v>
       </c>
     </row>
-    <row r="16" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:73" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>12</v>
       </c>
@@ -29442,7 +29447,7 @@
         <v>0.2111128591636503</v>
       </c>
     </row>
-    <row r="17" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>13</v>
       </c>
@@ -29660,7 +29665,7 @@
         <v>0.16216330057102221</v>
       </c>
     </row>
-    <row r="18" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>14</v>
       </c>
@@ -29830,7 +29835,7 @@
         <v>0.64272130707154407</v>
       </c>
     </row>
-    <row r="19" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>15</v>
       </c>
@@ -30048,7 +30053,7 @@
         <v>0.22684399283769241</v>
       </c>
     </row>
-    <row r="20" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -30266,7 +30271,7 @@
         <v>0.17901740747656539</v>
       </c>
     </row>
-    <row r="21" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -30484,7 +30489,7 @@
         <v>0.10449771543471691</v>
       </c>
     </row>
-    <row r="22" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -30702,7 +30707,7 @@
         <v>0.2743069571236858</v>
       </c>
     </row>
-    <row r="23" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>19</v>
       </c>
@@ -30920,7 +30925,7 @@
         <v>8.3028814784920302E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>20</v>
       </c>
@@ -31090,7 +31095,7 @@
         <v>0.62047597009617406</v>
       </c>
     </row>
-    <row r="25" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>21</v>
       </c>
@@ -31260,7 +31265,7 @@
         <v>0.84087800993271011</v>
       </c>
     </row>
-    <row r="26" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>22</v>
       </c>
@@ -31430,7 +31435,7 @@
         <v>0.57001248783600134</v>
       </c>
     </row>
-    <row r="27" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>23</v>
       </c>
@@ -31648,7 +31653,7 @@
         <v>0.2009740055073273</v>
       </c>
     </row>
-    <row r="28" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>24</v>
       </c>
@@ -31866,7 +31871,7 @@
         <v>0.26265842995032918</v>
       </c>
     </row>
-    <row r="29" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>25</v>
       </c>
@@ -32084,7 +32089,7 @@
         <v>9.3990636130204266E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>26</v>
       </c>
@@ -32302,7 +32307,7 @@
         <v>0.14697728660362841</v>
       </c>
     </row>
-    <row r="31" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>27</v>
       </c>
@@ -32472,7 +32477,7 @@
         <v>0.71093547687742764</v>
       </c>
     </row>
-    <row r="32" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>28</v>
       </c>
@@ -32690,7 +32695,7 @@
         <v>0.1225144100843169</v>
       </c>
     </row>
-    <row r="33" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>29</v>
       </c>
@@ -32908,7 +32913,7 @@
         <v>0.23081224152966209</v>
       </c>
     </row>
-    <row r="34" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>30</v>
       </c>
@@ -33078,7 +33083,7 @@
         <v>0.83425642525687471</v>
       </c>
     </row>
-    <row r="35" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>31</v>
       </c>
@@ -33296,7 +33301,7 @@
         <v>9.3548284717783911E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>32</v>
       </c>
@@ -33514,7 +33519,7 @@
         <v>0.1254756481945265</v>
       </c>
     </row>
-    <row r="37" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>33</v>
       </c>
@@ -33732,7 +33737,7 @@
         <v>0.21575216817004819</v>
       </c>
     </row>
-    <row r="38" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>34</v>
       </c>
@@ -33950,7 +33955,7 @@
         <v>0.13671950810937589</v>
       </c>
     </row>
-    <row r="39" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>35</v>
       </c>
@@ -34168,7 +34173,7 @@
         <v>0.1092833876121287</v>
       </c>
     </row>
-    <row r="40" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>36</v>
       </c>
@@ -34386,7 +34391,7 @@
         <v>0.15728321627368491</v>
       </c>
     </row>
-    <row r="41" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>37</v>
       </c>
@@ -34604,7 +34609,7 @@
         <v>0.24352283901274091</v>
       </c>
     </row>
-    <row r="42" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>38</v>
       </c>
@@ -34822,7 +34827,7 @@
         <v>0.19870870456991799</v>
       </c>
     </row>
-    <row r="43" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>39</v>
       </c>
@@ -35040,7 +35045,7 @@
         <v>0.14364989811362741</v>
       </c>
     </row>
-    <row r="44" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>40</v>
       </c>
@@ -35258,7 +35263,7 @@
         <v>0.12772077538916329</v>
       </c>
     </row>
-    <row r="45" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>41</v>
       </c>
@@ -35428,7 +35433,7 @@
         <v>0.68400647595518127</v>
       </c>
     </row>
-    <row r="46" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>42</v>
       </c>
@@ -35646,7 +35651,7 @@
         <v>0.10091229962882881</v>
       </c>
     </row>
-    <row r="47" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>43</v>
       </c>
@@ -35864,7 +35869,7 @@
         <v>0.1032139681166943</v>
       </c>
     </row>
-    <row r="48" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>44</v>
       </c>
@@ -36082,7 +36087,7 @@
         <v>8.9990308588674212E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>45</v>
       </c>
@@ -36300,7 +36305,7 @@
         <v>0.101579578422552</v>
       </c>
     </row>
-    <row r="50" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>46</v>
       </c>
@@ -36518,7 +36523,7 @@
         <v>0.1179680789376872</v>
       </c>
     </row>
-    <row r="51" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>47</v>
       </c>
@@ -36736,7 +36741,7 @@
         <v>0.16788377491993739</v>
       </c>
     </row>
-    <row r="52" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>48</v>
       </c>
@@ -36954,7 +36959,7 @@
         <v>0.14013253646281601</v>
       </c>
     </row>
-    <row r="53" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>49</v>
       </c>
@@ -37172,7 +37177,7 @@
         <v>0.1622098128033512</v>
       </c>
     </row>
-    <row r="54" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>50</v>
       </c>
@@ -37390,7 +37395,7 @@
         <v>0.11236381517047001</v>
       </c>
     </row>
-    <row r="55" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>51</v>
       </c>
@@ -37608,7 +37613,7 @@
         <v>9.4578293732735477E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>52</v>
       </c>
@@ -37778,7 +37783,7 @@
         <v>0.78067588303234059</v>
       </c>
     </row>
-    <row r="57" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>53</v>
       </c>
@@ -37996,7 +38001,7 @@
         <v>0.1139088904661661</v>
       </c>
     </row>
-    <row r="58" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>54</v>
       </c>
@@ -38214,7 +38219,7 @@
         <v>0.1680894637725332</v>
       </c>
     </row>
-    <row r="59" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>55</v>
       </c>
@@ -38384,7 +38389,7 @@
         <v>0.55471498609717163</v>
       </c>
     </row>
-    <row r="60" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>56</v>
       </c>
@@ -38602,7 +38607,7 @@
         <v>0.17684571587373221</v>
       </c>
     </row>
-    <row r="61" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>57</v>
       </c>
@@ -38820,7 +38825,7 @@
         <v>0.23216099233799001</v>
       </c>
     </row>
-    <row r="62" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>58</v>
       </c>
@@ -39038,7 +39043,7 @@
         <v>0.188498363572424</v>
       </c>
     </row>
-    <row r="63" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>59</v>
       </c>
@@ -39256,7 +39261,7 @@
         <v>0.1816704030786041</v>
       </c>
     </row>
-    <row r="64" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>60</v>
       </c>
@@ -39474,7 +39479,7 @@
         <v>0.1276580113156657</v>
       </c>
     </row>
-    <row r="65" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>61</v>
       </c>
@@ -39692,7 +39697,7 @@
         <v>0.1006830022692239</v>
       </c>
     </row>
-    <row r="66" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>62</v>
       </c>
@@ -39910,7 +39915,7 @@
         <v>0.19729022844511801</v>
       </c>
     </row>
-    <row r="67" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>63</v>
       </c>
@@ -40128,7 +40133,7 @@
         <v>0.17266344025956221</v>
       </c>
     </row>
-    <row r="68" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>64</v>
       </c>
@@ -40346,7 +40351,7 @@
         <v>0.17435696669449879</v>
       </c>
     </row>
-    <row r="69" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>65</v>
       </c>
@@ -40564,7 +40569,7 @@
         <v>0.1983227017475078</v>
       </c>
     </row>
-    <row r="70" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>66</v>
       </c>
@@ -40782,7 +40787,7 @@
         <v>0.14117684281039611</v>
       </c>
     </row>
-    <row r="71" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>67</v>
       </c>
@@ -41000,7 +41005,7 @@
         <v>0.1234837073662962</v>
       </c>
     </row>
-    <row r="72" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>68</v>
       </c>
@@ -41218,7 +41223,7 @@
         <v>0.2679768582242868</v>
       </c>
     </row>
-    <row r="73" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>69</v>
       </c>
@@ -41436,7 +41441,7 @@
         <v>0.1048487105948102</v>
       </c>
     </row>
-    <row r="74" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>70</v>
       </c>
@@ -41654,7 +41659,7 @@
         <v>0.2051699364951759</v>
       </c>
     </row>
-    <row r="75" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>71</v>
       </c>
@@ -41872,7 +41877,7 @@
         <v>9.0102274845784244E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>72</v>
       </c>
@@ -42090,7 +42095,7 @@
         <v>0.14411356825324159</v>
       </c>
     </row>
-    <row r="77" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>73</v>
       </c>
@@ -42260,7 +42265,7 @@
         <v>0.71817873818926026</v>
       </c>
     </row>
-    <row r="78" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>74</v>
       </c>
@@ -42430,7 +42435,7 @@
         <v>0.8068005596452672</v>
       </c>
     </row>
-    <row r="79" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>75</v>
       </c>
@@ -42600,7 +42605,7 @@
         <v>0.58276530228756784</v>
       </c>
     </row>
-    <row r="80" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>76</v>
       </c>
@@ -42818,7 +42823,7 @@
         <v>0.11234661590411869</v>
       </c>
     </row>
-    <row r="81" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>77</v>
       </c>
@@ -42988,7 +42993,7 @@
         <v>0.77469276002784548</v>
       </c>
     </row>
-    <row r="82" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>78</v>
       </c>
@@ -43206,7 +43211,7 @@
         <v>0.12408589670803261</v>
       </c>
     </row>
-    <row r="83" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>79</v>
       </c>
@@ -43424,7 +43429,7 @@
         <v>0.1610423628942261</v>
       </c>
     </row>
-    <row r="84" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>80</v>
       </c>
@@ -43594,7 +43599,7 @@
         <v>0.6774140670528197</v>
       </c>
     </row>
-    <row r="85" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>81</v>
       </c>
@@ -43812,7 +43817,7 @@
         <v>0.1581055050705239</v>
       </c>
     </row>
-    <row r="86" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>82</v>
       </c>
@@ -44030,7 +44035,7 @@
         <v>0.11622875274421821</v>
       </c>
     </row>
-    <row r="87" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>83</v>
       </c>
@@ -44248,7 +44253,7 @@
         <v>0.14220681913133809</v>
       </c>
     </row>
-    <row r="88" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>84</v>
       </c>
@@ -44466,7 +44471,7 @@
         <v>0.1149483015808594</v>
       </c>
     </row>
-    <row r="89" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>85</v>
       </c>
@@ -44684,7 +44689,7 @@
         <v>0.1118161581911726</v>
       </c>
     </row>
-    <row r="90" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>86</v>
       </c>
@@ -44902,7 +44907,7 @@
         <v>0.20812621466964801</v>
       </c>
     </row>
-    <row r="91" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>87</v>
       </c>
@@ -45120,7 +45125,7 @@
         <v>0.1022603319243419</v>
       </c>
     </row>
-    <row r="92" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>88</v>
       </c>
@@ -45338,7 +45343,7 @@
         <v>0.21790701206565419</v>
       </c>
     </row>
-    <row r="93" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>89</v>
       </c>
@@ -45556,7 +45561,7 @@
         <v>0.18663929758296821</v>
       </c>
     </row>
-    <row r="94" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>90</v>
       </c>
@@ -45774,7 +45779,7 @@
         <v>0.14301576873436739</v>
       </c>
     </row>
-    <row r="95" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>91</v>
       </c>
@@ -45992,7 +45997,7 @@
         <v>0.1005257080430314</v>
       </c>
     </row>
-    <row r="96" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>92</v>
       </c>
@@ -46210,7 +46215,7 @@
         <v>9.6315755367863701E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>93</v>
       </c>
@@ -46428,7 +46433,7 @@
         <v>9.8490784235466949E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>94</v>
       </c>
@@ -46646,7 +46651,7 @@
         <v>0.17179850904250879</v>
       </c>
     </row>
-    <row r="99" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>95</v>
       </c>
@@ -46864,7 +46869,7 @@
         <v>0.2234466857253809</v>
       </c>
     </row>
-    <row r="100" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>96</v>
       </c>
@@ -47082,7 +47087,7 @@
         <v>0.19210161020711361</v>
       </c>
     </row>
-    <row r="101" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>97</v>
       </c>
@@ -47300,7 +47305,7 @@
         <v>0.19378256717234951</v>
       </c>
     </row>
-    <row r="102" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>98</v>
       </c>
@@ -47470,7 +47475,7 @@
         <v>0.61795412962363194</v>
       </c>
     </row>
-    <row r="103" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>99</v>
       </c>
@@ -47690,26 +47695,26 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="AA1:AB1"/>
+    <mergeCell ref="AC1:AD1"/>
+    <mergeCell ref="AE1:AF1"/>
+    <mergeCell ref="AI1:AJ1"/>
+    <mergeCell ref="AK1:AL1"/>
+    <mergeCell ref="AN1:AO1"/>
     <mergeCell ref="AR1:AS1"/>
     <mergeCell ref="AT1:AU1"/>
     <mergeCell ref="AV1:AY1"/>
     <mergeCell ref="AZ1:BD1"/>
     <mergeCell ref="BE1:BU1"/>
-    <mergeCell ref="AC1:AD1"/>
-    <mergeCell ref="AE1:AF1"/>
-    <mergeCell ref="AI1:AJ1"/>
-    <mergeCell ref="AK1:AL1"/>
-    <mergeCell ref="AN1:AO1"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="AA1:AB1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>